<commit_message>
Spatial pattern tests operational
Removed data

Reduce test files sized so lfs is no longer needed

Remove dead code
</commit_message>
<xml_diff>
--- a/logic/test/data/spatialinventory/bef/reporting_2021/2000/Emissies per km2 excl puntbrongegevens_2000_CO.xlsx
+++ b/logic/test/data/spatialinventory/bef/reporting_2021/2000/Emissies per km2 excl puntbrongegevens_2000_CO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RMABuild\emap\logic\test\data\spatialinventory\bef\reporting_2021\2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RMABuild\emap\logic\test\data\spatialinventory\bef\reporting_2021\2000\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C755DC9D-02E9-4A0A-88A2-A63CC55814A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00480147-0D7A-41F2-94FA-CAA715E8047E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3684" yWindow="3180" windowWidth="24540" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019_PM2.5" sheetId="1" r:id="rId1"/>
@@ -375,20 +375,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="1" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -409,6 +409,11 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>
@@ -418,5 +423,6 @@
     <sortCondition ref="E2:E355997"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>